<commit_message>
Added new parameter for specifying APRX locations
User's can either provide the tool with a single directory path that contains all APRX files, or users can continue using the APRX_PATH column within the PDFMultiExport.xlsx spreadsheet. The single directory path option gives GISS in a multi-user environment the ability to all use the same PDFMultiExport.xlsx spreadsheet.
</commit_message>
<xml_diff>
--- a/PDFMultiExport.xlsx
+++ b/PDFMultiExport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\development\PanunTools-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C84FA4F-671F-4844-A102-47B079E4388D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AAFA8C-F083-4978-AE34-3CC27278992E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="121">
   <si>
     <t>PRODUCTS_DATE</t>
   </si>
@@ -363,6 +363,42 @@
   <si>
     <t>EXPORT_REQUEST_LABEL</t>
   </si>
+  <si>
+    <t>airops_2021_Windy_CATIA003058_ArcPro_2_7.aprx</t>
+  </si>
+  <si>
+    <t>brief_2021_Windy_CATIA003058_ArcPro_2_7.aprx</t>
+  </si>
+  <si>
+    <t>iap_2021_Windy_CATIA003058_ArcPro_2_7.aprx</t>
+  </si>
+  <si>
+    <t>ops_2021_Windy_CATIA003058_ArcPro_2_7.aprx</t>
+  </si>
+  <si>
+    <t>owner_2021_Windy_CATIA003058_ArcPro_2_7.aprx</t>
+  </si>
+  <si>
+    <t>pilot_2021_Windy_CATIA003058_ArcPro_2_7.aprx</t>
+  </si>
+  <si>
+    <t>pio_2021_Windy_CATIA003058_ArcPro_2_7.aprx</t>
+  </si>
+  <si>
+    <t>prog_2021_Windy_CATIA003058_ArcPro_2_7.aprx</t>
+  </si>
+  <si>
+    <t>repair_2021_Windy_CATIA003058_ArcPro_2_7.aprx</t>
+  </si>
+  <si>
+    <t>repair_tiles_2021_Windy_CATIA003058_ArcPro_2_7.aprx</t>
+  </si>
+  <si>
+    <t>trans_2021_Windy_CATIA003058_ArcPro_2_7.aprx</t>
+  </si>
+  <si>
+    <t>APRX_FILENAME</t>
+  </si>
 </sst>
 </file>
 
@@ -498,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -783,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C5D0DF9-225F-4A6B-A31B-C4BC4EBA5000}">
-  <dimension ref="A1:AB987"/>
+  <dimension ref="A1:AC987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB24" sqref="AB24"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -818,10 +854,11 @@
     <col min="25" max="25" width="18.375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="77.375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="105.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="45.125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="105.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>57</v>
       </c>
@@ -904,10 +941,13 @@
         <v>4</v>
       </c>
       <c r="AB1" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC1" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -982,10 +1022,13 @@
         <v>73</v>
       </c>
       <c r="AB2" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC2" s="24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -1060,10 +1103,13 @@
         <v>73</v>
       </c>
       <c r="AB3" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC3" s="24" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>38</v>
       </c>
@@ -1134,10 +1180,13 @@
         <v>76</v>
       </c>
       <c r="AB4" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC4" s="24" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>38</v>
       </c>
@@ -1212,10 +1261,13 @@
         <v>73</v>
       </c>
       <c r="AB5" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC5" s="24" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>38</v>
       </c>
@@ -1290,10 +1342,13 @@
         <v>73</v>
       </c>
       <c r="AB6" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC6" s="24" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
@@ -1368,10 +1423,13 @@
         <v>76</v>
       </c>
       <c r="AB7" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC7" s="24" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
@@ -1446,10 +1504,13 @@
         <v>73</v>
       </c>
       <c r="AB8" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC8" s="24" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>38</v>
       </c>
@@ -1524,10 +1585,13 @@
         <v>85</v>
       </c>
       <c r="AB9" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC9" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
@@ -1602,10 +1666,13 @@
         <v>73</v>
       </c>
       <c r="AB10" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC10" s="24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>38</v>
       </c>
@@ -1679,10 +1746,13 @@
         <v>76</v>
       </c>
       <c r="AB11" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC11" s="24" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>38</v>
       </c>
@@ -1757,10 +1827,13 @@
         <v>73</v>
       </c>
       <c r="AB12" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC12" s="24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1784,7 +1857,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1808,7 +1881,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1832,7 +1905,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>

</xml_diff>

<commit_message>
Added JPEG2000 image compression option
</commit_message>
<xml_diff>
--- a/PDFMultiExport.xlsx
+++ b/PDFMultiExport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\development\PanunTools-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AAFA8C-F083-4978-AE34-3CC27278992E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C48AEA0-BA6D-45E6-B325-D933D045A95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="122">
   <si>
     <t>PRODUCTS_DATE</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>APRX_FILENAME</t>
+  </si>
+  <si>
+    <t>JPEG2000</t>
   </si>
 </sst>
 </file>
@@ -821,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C5D0DF9-225F-4A6B-A31B-C4BC4EBA5000}">
   <dimension ref="A1:AC987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1707,9 +1710,8 @@
       <c r="N11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="19" t="str">
-        <f t="shared" ref="O11" si="0">"ADAPTIVE"</f>
-        <v>ADAPTIVE</v>
+      <c r="O11" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="P11" s="19">
         <v>80</v>
@@ -28197,12 +28199,6 @@
           </x14:formula1>
           <xm:sqref>N2:N12 Q2:Q12 T2:T12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E635C8B7-A510-4D5E-B49B-10C9EE291C37}">
-          <x14:formula1>
-            <xm:f>ValueLists!$E$2:$E$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>O2:O12</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BAF5E788-246B-4720-836F-9DF4373F6D58}">
           <x14:formula1>
             <xm:f>ValueLists!$D$2:$D$6</xm:f>
@@ -28215,6 +28211,12 @@
           </x14:formula1>
           <xm:sqref>U2:U12</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1FF79BA4-7505-4422-B82C-102CB009DB55}">
+          <x14:formula1>
+            <xm:f>ValueLists!$E$2:$E$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:O12</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -28226,7 +28228,7 @@
   <dimension ref="A1:U1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28412,8 +28414,8 @@
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>23</v>
+      <c r="E5" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -28441,7 +28443,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -28465,7 +28467,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -28488,7 +28490,9 @@
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>

</xml_diff>